<commit_message>
git all doc may.20
</commit_message>
<xml_diff>
--- a/Django/docs.djangoproject.com.xlsx
+++ b/Django/docs.djangoproject.com.xlsx
@@ -1281,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C9:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>

</xml_diff>